<commit_message>
updated files into repo
</commit_message>
<xml_diff>
--- a/Documents/ML Phishing Papers.xlsx
+++ b/Documents/ML Phishing Papers.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moldy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moldy/Desktop/GitProjects/ML.PhishingEmailDetection/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8630E222-411A-5E49-8A64-0044E05F86AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F7A182-B074-7046-9921-395DF3EFBF5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EA6C9B02-2554-5043-9163-EC39B644AC4E}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" activeTab="1" xr2:uid="{EA6C9B02-2554-5043-9163-EC39B644AC4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Featureas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="156">
   <si>
     <t>https://ieeexplore.ieee.org/abstract/document/8004877</t>
   </si>
@@ -1129,6 +1130,108 @@
   </si>
   <si>
     <t>improved detection by implementing malicious features ates for C4.5, MLP, Naïve Bayer and Random Forest were also improved by 4%, 25%, 17% and 2% respectively.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header </t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Syntactic Struct: access click confirm enter follow protect update use</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Feature Words used in SAFe-PC:</t>
+  </si>
+  <si>
+    <t>able, access, account, accounts, action, activate, activated, activation, active, activities, admin, administrator, advise, alert, alerts, allie, allied, allow, alt, alternative, animal, answered, anti, anything, apologize, asthma, attach, attached, attachment, attempt, attention, authorize, aware, away, back, balance, bank, banking, banks, banner, believe, best, better, beyond, bill, biz, blackboard, blog, canada, canopy, captain, card, cards, care, cars, carson, cervices, change, changed, check, chief, children, choosing, chord, click, clicking, college, complete, computer, confirm, confirmation, continue, convenient, correct, correctly, could, credit, creek, critical, customer, customers, daly, dangerous, dari, data, days, deactivate, deactivated, dear, decline, department, depression, description, details, different, digital, dir, dire, direct, director, disposition, doctor, document, domain, double, due, easy, effective, email, emails, ensure, error, even, every, everything, executive, expire, failure, fastest, feature, federally, filelocker, filename, financing, find, finder, first, following, food, found, frank, franklin, fraud, freeze, full, function, gallery, get, good, got, gothic, greg, group, growth, hammad, head, head, hello, help, helpful, hen, high, hold, honda, however, husky, identify, images, immediately, important, inc, includes, inconvenience, incorrect, ind, individuals, information, interruption, invoicing, issue, itap, kindly, know, latest, lead, learn, legal, let, letting, life, like, lin, link, locked, lodge, log, logging, logo, logos, long, longer, mai, mail, main, maintenance, make, making, mall, man, managing, many, marks, may, media, medium, member, men, message, method, minimum, miss, mistake, mobile, mohammad, monday, monitored, month, monthly, moodle, much, multiple, need, needed, never, new, notice, notification, number, officer, often, oil, okay, one, operation, pack, page, pain, passion, paul, pay, paying, payment, payments, people, peoplesoft, phone, photo, please, point, policy, power, present, primary, problem, problems, proceed, process, professional, profile, prompt, protect, protection, proxy, questions, reach, reader, really, reasons, receive, recently, redirect, reed, register, registered, rel, repayment, reply, request, requested, require, reset, resolve, respond, restore, reverse, right, riley, risk, roman, rural, safeguard, safety, said, school, scripts, secure, securely, security, see, send, sent, serious, server, service, services, settings, several, sex, shelter, show, signin, sincerely, site, society, soft, something, standard, statement, still, strong, strongly, subject, super, sure, suspend, suspended, suspension, tab, take, target, team, technical, texts, thank, thanks, think, throat, time, times, title, today, took, toyota, transfers, treatment, trust, try, two, ufa, ultimate, unable, unauthorized, university, unpaid, unusual, update, updated, upgraded, uploads, urgent, use, user, username, using, validate, value, verification, verify, version, via, view, voice, want, way, website, well, wishes, without, work, working, world, would, [Purdue Mascot 1], [Purdue Mascot 2], [Indiana], [West Lafayette], [Purdue University], [Purdue University Portal], and [Purdue University Payroll].</t>
+  </si>
+  <si>
+    <t>char and word vectors RCNN model</t>
+  </si>
+  <si>
+    <t>Char and word vectors RCNN model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BlackListed Words: </t>
+  </si>
+  <si>
+    <t>Account access bank credit quick identity verify limit statement restrict inconvenience information limited log minutes password debit update user client recently risk social security service suspension suspended member confirm hold</t>
+  </si>
+  <si>
+    <t>word2vec embedding to capture synaptic and semantic similarity of phishing emails</t>
+  </si>
+  <si>
+    <t>SubjectVerifyWord</t>
+  </si>
+  <si>
+    <t>SubjectNumChars</t>
+  </si>
+  <si>
+    <t>Textmail (New)</t>
+  </si>
+  <si>
+    <t>SubjectNumWords</t>
+  </si>
+  <si>
+    <t>MultiPartMail (New)</t>
+  </si>
+  <si>
+    <t>SubjectRichness</t>
+  </si>
+  <si>
+    <t>SendNumWords</t>
+  </si>
+  <si>
+    <t>SendDiffReplayto</t>
+  </si>
+  <si>
+    <t>SubjectBankWord</t>
+  </si>
+  <si>
+    <t>SubjectDebitWord</t>
+  </si>
+  <si>
+    <t>SubjectFwdWord</t>
+  </si>
+  <si>
+    <t>SizeOfDocument</t>
+  </si>
+  <si>
+    <t>BodyRichness</t>
+  </si>
+  <si>
+    <t>BodyDearWord</t>
+  </si>
+  <si>
+    <t>BodyNumFunctionWords</t>
+  </si>
+  <si>
+    <t>BodyNumChars</t>
+  </si>
+  <si>
+    <t>BodySuspensionWord</t>
+  </si>
+  <si>
+    <t>BodyNumWords</t>
+  </si>
+  <si>
+    <t>BodyVerifyYourAccountPhrase</t>
+  </si>
+  <si>
+    <t>BodyNumUniqueWords</t>
+  </si>
+  <si>
+    <t>VERBS</t>
+  </si>
+  <si>
+    <t>bring, change, check, complete, confirm, create, enter, find, give, make, open, pay, protect, provide, receive, remove, review, sign, update, buy, visit, win, delete, approve, set, lose, submit, renew, replace, acquire, obtain, purchase, click, verify, earn, release, share, deposit, activate, reactivate, reconfirm, register, download, withdraw, access, assist, fill, secure, validate, deliver, transfer, discuss, attach, schedule, raise, build, file, consider, reduce, kill, investigate.</t>
   </si>
 </sst>
 </file>
@@ -1136,9 +1239,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1222,8 +1325,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1233,6 +1342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1251,7 +1366,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1263,14 +1378,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1299,6 +1414,10 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1354,7 +1473,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4914899" y="3987800"/>
+          <a:off x="4912013" y="3989532"/>
           <a:ext cx="939801" cy="881924"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1373,9 +1492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
+      <xdr:colOff>711200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>3149600</xdr:rowOff>
+      <xdr:rowOff>2809937</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1405,7 +1524,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1587500" y="24333200"/>
-          <a:ext cx="2590800" cy="3149600"/>
+          <a:ext cx="2311400" cy="2809937"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1454,8 +1573,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3403600" y="36220401"/>
-          <a:ext cx="2184400" cy="393699"/>
+          <a:off x="3412797" y="36273391"/>
+          <a:ext cx="2192720" cy="393699"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1816,9 +1935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D7F45B-88A6-934C-B723-B7341C10A6C3}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+    <sheetView zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1870,7 +1989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="170">
+    <row r="3" spans="1:6" ht="187">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1910,7 +2029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="272">
+    <row r="5" spans="1:6" ht="289">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
@@ -1920,7 +2039,7 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="19" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="5">
@@ -1940,7 +2059,7 @@
       <c r="C6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="19" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1969,7 +2088,7 @@
       <c r="C8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="19" t="s">
         <v>37</v>
       </c>
       <c r="E8" s="5">
@@ -1979,7 +2098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="153">
+    <row r="9" spans="1:6" ht="170">
       <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
@@ -2027,7 +2146,7 @@
         <v>50</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="19" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -2047,7 +2166,7 @@
       <c r="C12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -2084,7 +2203,7 @@
       <c r="C14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="19" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -2140,7 +2259,7 @@
       <c r="C17" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="19" t="s">
         <v>76</v>
       </c>
       <c r="E17" s="5"/>
@@ -2158,7 +2277,7 @@
       <c r="C18" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="19" t="s">
         <v>82</v>
       </c>
       <c r="E18" s="5">
@@ -2201,7 +2320,7 @@
         <v>90</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="19" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="5">
@@ -2217,7 +2336,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="19" t="s">
         <v>93</v>
       </c>
       <c r="E22" s="5"/>
@@ -2418,4 +2537,156 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId27"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2B0FB0-EBCF-324C-ADE5-AC75BCE5D7AC}">
+  <dimension ref="B2:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>